<commit_message>
Update Data driven Add Contacts method
</commit_message>
<xml_diff>
--- a/FreeCRMTest/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/FreeCRMTest/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -34,10 +34,10 @@
     <t>title</t>
   </si>
   <si>
-    <t>fName</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>lName</t>
+    <t>Surname</t>
   </si>
   <si>
     <t>Dr.</t>
@@ -1234,7 +1234,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2"/>

</xml_diff>